<commit_message>
ques addition issue resolved
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -424,22 +424,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>topic_id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>topic</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>question</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>url</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -456,54 +456,54 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>b20834b6149c11ee8154b182d7ced985</t>
+          <t>abcd</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>fc1c3f36164311eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>arrays</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Path Sum II</t>
-        </is>
-      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://leetcode.com/problems/path-sum-ii/</t>
+          <t>asdf</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>medium</t>
+          <t>easy</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>leetcode</t>
+          <t>codechef</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>a173671c15d011ee8e788d805d81dcbd</t>
+          <t>adcde</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>55c324b8164511eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>twoPointers</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>sadawd</t>
-        </is>
-      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>asdasd</t>
+          <t>sadd</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">

</xml_diff>

<commit_message>
table data api done
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -677,6 +677,518 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/target-sum/?envType=list&amp;envId=er2c1j13</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>8c186c94199711eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>arrays</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Target Sum</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>leetcode</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/maximum-sum-circular-subarray/?envType=list&amp;envId=er2c1j13</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>9e6b97e0199711eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>arrays</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Maximum Sum Circular Subarray</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>leetcode</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/longest-substring-without-repeating-characters/?envType=list&amp;envId=efdk2wsi</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>bfcc797c199711eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>strings</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Longest Substring Without Repeating Characters</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>leetcode</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/longest-palindromic-substring/?envType=list&amp;envId=efdk2wsi</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>d317bc62199711eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>strings</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Longest Palindromic Substring</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>leetcode</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/decode-string/?envType=list&amp;envId=efdk2wsi</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>dfdd21da199711eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>strings</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Decode String</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>leetcode</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/longest-common-prefix/?envType=list&amp;envId=efdk2wsi</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>072e0b1e199811eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>strings</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Longest Common Prefix</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>leetcode</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/repeated-substring-pattern/?envType=list&amp;envId=efdk2wsi</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>36ff972c199811eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>strings</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Repeated Substring Pattern</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>leetcode</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/sort-characters-by-frequency/?envType=list&amp;envId=efdk2wsi</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>4cb30a90199811eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>strings</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Sort Characters By Frequency</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>leetcode</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/longest-duplicate-substring/?envType=list&amp;envId=efdk2wsi</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>6742bc0c199811eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>strings</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Longest Duplicate Substring</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>hard</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>leetcode</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/reformat-the-string/?envType=list&amp;envId=efdk2wsi</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>77897c90199811eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>strings</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Reformat The String</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>leetcode</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/split-two-strings-to-make-palindrome/</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>e71f12f4199811eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>twoPointers</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Split Two Strings to Make Palindrome</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>leetcode</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/3sum/</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>f5df63a2199811eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>twoPointers</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>3Sum</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>leetcode</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/shortest-unsorted-continuous-subarray/</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>0759382e199911eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>twoPointers</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Shortest Unsorted Continuous Subarray</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>leetcode</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/rotate-array/</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>14bc1a04199911eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>twoPointers</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Rotate Array</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>leetcode</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/next-permutation/</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>374ca1d8199911eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>twoPointers</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Next Permutation</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>leetcode</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>https://leetcode.com/problems/squares-of-a-sorted-array/</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>535cf4c2199911eea88ae3300d621ca4</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>twoPointers</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Squares of a Sorted Array</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>leetcode</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>